<commit_message>
added Rdotnet to methods.
</commit_message>
<xml_diff>
--- a/testRAddin.xlsx
+++ b/testRAddin.xlsx
@@ -14,27 +14,27 @@
   <sheets>
     <sheet name="Main Test" sheetId="1" r:id="rId1"/>
     <sheet name="Test_scriptRng" sheetId="7" r:id="rId2"/>
-    <sheet name="Test_Toy" sheetId="5" r:id="rId3"/>
+    <sheet name="Test_OtherSheet" sheetId="5" r:id="rId3"/>
     <sheet name="Test_RdotNet" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="R_Addin" localSheetId="2">Test_OtherSheet!$J$1:$L$5</definedName>
     <definedName name="R_Addin" localSheetId="3">Test_RdotNet!$A$1:$C$6</definedName>
-    <definedName name="R_Addin" localSheetId="2">Test_Toy!$J$1:$L$5</definedName>
     <definedName name="R_Addin">'Main Test'!$J$1:$L$5</definedName>
-    <definedName name="R_AddinAnotherDef" localSheetId="2">Test_Toy!$J$7:$L$12</definedName>
+    <definedName name="R_AddinAnotherDef" localSheetId="2">Test_OtherSheet!$J$7:$L$12</definedName>
     <definedName name="R_AddinAnotherDef">'Main Test'!$M$1:$O$5</definedName>
     <definedName name="R_AddinScriptCell" localSheetId="1">Test_scriptRng!$A$25:$C$29</definedName>
     <definedName name="R_AddinScriptRange" localSheetId="1">Test_scriptRng!$A$19:$C$23</definedName>
     <definedName name="scriptRange" localSheetId="1">Test_scriptRng!$B$1:$B$17</definedName>
+    <definedName name="test_in" localSheetId="2">Test_OtherSheet!$B$1:$H$4</definedName>
     <definedName name="test_in" localSheetId="3">Test_RdotNet!$A$9:$A$14</definedName>
-    <definedName name="test_in" localSheetId="2">Test_Toy!$B$1:$H$4</definedName>
     <definedName name="test_in">'Main Test'!$B$1:$H$301</definedName>
+    <definedName name="test_out" localSheetId="2">Test_OtherSheet!$A$2:$A$4</definedName>
     <definedName name="test_out" localSheetId="3">Test_RdotNet!$B$9:$B$14</definedName>
-    <definedName name="test_out" localSheetId="2">Test_Toy!$A$2:$A$4</definedName>
     <definedName name="test_out">'Main Test'!$A$2:$A$49</definedName>
+    <definedName name="testdiagram" localSheetId="2">Test_OtherSheet!$J$17</definedName>
     <definedName name="testdiagram" localSheetId="3">Test_RdotNet!$D$2</definedName>
     <definedName name="testdiagram" localSheetId="1">Test_scriptRng!$D$2</definedName>
-    <definedName name="testdiagram" localSheetId="2">Test_Toy!$J$17</definedName>
     <definedName name="testdiagram">'Main Test'!$J$8</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
@@ -192,15 +192,6 @@
     <t>scriptRange</t>
   </si>
   <si>
-    <t>Test_Toy!test_in</t>
-  </si>
-  <si>
-    <t>Test_Toy!test_out</t>
-  </si>
-  <si>
-    <t>Test_Toy!testdiagram</t>
-  </si>
-  <si>
     <t>Test_scriptRng!testdiagram</t>
   </si>
   <si>
@@ -232,6 +223,15 @@
   </si>
   <si>
     <t>C:\Program Files\R\R-3.4.0\bin\i386</t>
+  </si>
+  <si>
+    <t>Test_OtherSheet!test_in</t>
+  </si>
+  <si>
+    <t>Test_OtherSheet!test_out</t>
+  </si>
+  <si>
+    <t>Test_OtherSheet!testdiagram</t>
   </si>
 </sst>
 </file>
@@ -8497,7 +8497,7 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C23"/>
       <c r="D23"/>
@@ -14685,7 +14685,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14772,14 +14772,14 @@
         <v>3</v>
       </c>
       <c r="C3" t="str">
-        <f>IFERROR(IF(D3=0,CODE(RIGHT(Test_Toy!#REF!,LEN(Test_Toy!#REF!)-1))-64,CODE(Test_Toy!#REF!)-64),"")</f>
+        <f>IFERROR(IF(D3=0,CODE(RIGHT(Test_OtherSheet!#REF!,LEN(Test_OtherSheet!#REF!)-1))-64,CODE(Test_OtherSheet!#REF!)-64),"")</f>
         <v/>
       </c>
       <c r="D3">
         <v>3</v>
       </c>
       <c r="E3" t="str">
-        <f>IFERROR(IF(F3=0,CODE(RIGHT(Test_Toy!#REF!,LEN(Test_Toy!#REF!)-1))-64,CODE(Test_Toy!#REF!)-64),"")</f>
+        <f>IFERROR(IF(F3=0,CODE(RIGHT(Test_OtherSheet!#REF!,LEN(Test_OtherSheet!#REF!)-1))-64,CODE(Test_OtherSheet!#REF!)-64),"")</f>
         <v/>
       </c>
       <c r="F3">
@@ -14796,7 +14796,7 @@
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -14807,14 +14807,14 @@
         <v>3</v>
       </c>
       <c r="C4" t="str">
-        <f>IFERROR(IF(D4=0,CODE(RIGHT(Test_Toy!#REF!,LEN(Test_Toy!#REF!)-1))-64,CODE(Test_Toy!#REF!)-64),"")</f>
+        <f>IFERROR(IF(D4=0,CODE(RIGHT(Test_OtherSheet!#REF!,LEN(Test_OtherSheet!#REF!)-1))-64,CODE(Test_OtherSheet!#REF!)-64),"")</f>
         <v/>
       </c>
       <c r="D4">
         <v>3</v>
       </c>
       <c r="E4" t="str">
-        <f>IFERROR(IF(F4=0,CODE(RIGHT(Test_Toy!#REF!,LEN(Test_Toy!#REF!)-1))-64,CODE(Test_Toy!#REF!)-64),"")</f>
+        <f>IFERROR(IF(F4=0,CODE(RIGHT(Test_OtherSheet!#REF!,LEN(Test_OtherSheet!#REF!)-1))-64,CODE(Test_OtherSheet!#REF!)-64),"")</f>
         <v/>
       </c>
       <c r="F4">
@@ -14830,7 +14830,7 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -14839,7 +14839,7 @@
         <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -14879,7 +14879,7 @@
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -14888,7 +14888,7 @@
         <v>5</v>
       </c>
       <c r="K11" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -14897,7 +14897,7 @@
         <v>7</v>
       </c>
       <c r="K12" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -15039,10 +15039,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="165.75" x14ac:dyDescent="0.2">
@@ -15050,7 +15050,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -15058,7 +15058,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -15066,7 +15066,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -15074,7 +15074,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
split main vb into 3 classes improved rdotnet handling
</commit_message>
<xml_diff>
--- a/testRAddin.xlsx
+++ b/testRAddin.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="150" windowWidth="5040" windowHeight="7470"/>
+    <workbookView xWindow="15180" yWindow="150" windowWidth="5040" windowHeight="7470" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Main Test" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="R_Addin" localSheetId="2">Test_OtherSheet!$J$1:$L$5</definedName>
-    <definedName name="R_Addin" localSheetId="3">Test_RdotNet!$A$1:$C$6</definedName>
+    <definedName name="R_Addin" localSheetId="3">Test_RdotNet!$A$1:$C$7</definedName>
     <definedName name="R_Addin">'Main Test'!$J$1:$L$5</definedName>
     <definedName name="R_AddinAnotherDef" localSheetId="2">Test_OtherSheet!$J$7:$L$12</definedName>
     <definedName name="R_AddinAnotherDef">'Main Test'!$M$1:$O$5</definedName>
@@ -27,13 +27,14 @@
     <definedName name="R_AddinScriptRange" localSheetId="1">Test_scriptRng!$A$19:$C$23</definedName>
     <definedName name="scriptRange" localSheetId="1">Test_scriptRng!$B$1:$B$17</definedName>
     <definedName name="test_in" localSheetId="2">Test_OtherSheet!$B$1:$H$4</definedName>
-    <definedName name="test_in" localSheetId="3">Test_RdotNet!$A$9:$A$14</definedName>
+    <definedName name="test_in" localSheetId="3">Test_RdotNet!$E$1:$K$4</definedName>
     <definedName name="test_in">'Main Test'!$B$1:$H$301</definedName>
     <definedName name="test_out" localSheetId="2">Test_OtherSheet!$A$2:$A$4</definedName>
-    <definedName name="test_out" localSheetId="3">Test_RdotNet!$B$9:$B$14</definedName>
+    <definedName name="test_out" localSheetId="3">Test_RdotNet!$D$2:$D$4</definedName>
     <definedName name="test_out">'Main Test'!$A$2:$A$49</definedName>
+    <definedName name="test_out2" localSheetId="3">Test_RdotNet!$E$8</definedName>
     <definedName name="testdiagram" localSheetId="2">Test_OtherSheet!$J$17</definedName>
-    <definedName name="testdiagram" localSheetId="3">Test_RdotNet!$D$2</definedName>
+    <definedName name="testdiagram" localSheetId="3">Test_RdotNet!$A$10</definedName>
     <definedName name="testdiagram" localSheetId="1">Test_scriptRng!$D$2</definedName>
     <definedName name="testdiagram">'Main Test'!$J$8</definedName>
   </definedNames>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3672" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3692" uniqueCount="58">
   <si>
     <t/>
   </si>
@@ -207,24 +208,6 @@
     <t>Test_RdotNet!test_in</t>
   </si>
   <si>
-    <t>library(ggplot2)
-initial.options &lt;- commandArgs(trailingOnly = FALSE)
-script.name &lt;- sub("--file=", "", initial.options[grep("--file=", initial.options)])
-script.basename &lt;- dirname(script.name)
-if (length(script.basename) == 0) {
-  # this only works RGui
-  script.basename &lt;- getSrcDirectory(function(x) {x})
-}
-setwd(script.basename)
-gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()
-png(filename="testdiagram.png")
-print(gplot)
-dev.off()</t>
-  </si>
-  <si>
-    <t>C:\Program Files\R\R-3.4.0\bin\i386</t>
-  </si>
-  <si>
     <t>Test_OtherSheet!test_in</t>
   </si>
   <si>
@@ -232,6 +215,30 @@
   </si>
   <si>
     <t>Test_OtherSheet!testdiagram</t>
+  </si>
+  <si>
+    <t>C:\Program Files\Microsoft\MRO\R-3.3.2\bin</t>
+  </si>
+  <si>
+    <t>Test_RdotNet!test_out2</t>
+  </si>
+  <si>
+    <t>0,5</t>
+  </si>
+  <si>
+    <t>0,9</t>
+  </si>
+  <si>
+    <t>library(ggplot2)
+header &lt;- unlist(test_in[1,]) # the first row will be the header
+test_in &lt;- test_in[-1,]          # removing the first row.
+colnames(test_in) &lt;-header
+test_out &lt;- c(1,2,3) # test_in[,1]+20
+test_out2 &lt;- test_in #data.frame(sapply(test_in, function(x) as.numeric(as.character(x))))
+#gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()</t>
+  </si>
+  <si>
+    <t>0.8</t>
   </si>
 </sst>
 </file>
@@ -933,7 +940,7 @@
   <sheetPr codeName="eingabe"/>
   <dimension ref="A1:O301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
@@ -8226,7 +8233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M302"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -14685,7 +14692,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection sqref="A1:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14796,7 +14803,7 @@
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -14830,7 +14837,7 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -14839,7 +14846,7 @@
         <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -14879,7 +14886,7 @@
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -14888,7 +14895,7 @@
         <v>5</v>
       </c>
       <c r="K11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -14897,7 +14904,7 @@
         <v>7</v>
       </c>
       <c r="K12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -15018,50 +15025,150 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="63.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" customWidth="1"/>
+    <col min="4" max="11" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="165.75" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2" s="1">
+        <v>3</v>
+      </c>
+      <c r="K2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>500</v>
+      </c>
+      <c r="F3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3" t="str">
+        <f>IFERROR(IF(I3=0,CODE(RIGHT(Test_OtherSheet!#REF!,LEN(Test_OtherSheet!#REF!)-1))-64,CODE(Test_OtherSheet!#REF!)-64),"")</f>
+        <v/>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3" s="1">
+        <v>3</v>
+      </c>
+      <c r="K3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="20" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>300</v>
+      </c>
+      <c r="F4">
+        <v>0.9</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="str">
+        <f>IFERROR(IF(I4=0,CODE(RIGHT(Test_OtherSheet!#REF!,LEN(Test_OtherSheet!#REF!)-1))-64,CODE(Test_OtherSheet!#REF!)-64),"")</f>
+        <v/>
+      </c>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4" s="1">
+        <v>3</v>
+      </c>
+      <c r="K4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -15069,12 +15176,106 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B7" s="20" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" t="s">
+        <v>12</v>
+      </c>
+      <c r="K8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>100</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9">
+        <v>3</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9">
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>500</v>
+      </c>
+      <c r="F10">
+        <v>0.8</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>300</v>
+      </c>
+      <c r="F11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>3</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
improved error msg handling (you can now ignore further error messages or cancel the whole rdefinition run)
</commit_message>
<xml_diff>
--- a/testRAddin.xlsx
+++ b/testRAddin.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="150" windowWidth="5040" windowHeight="7470" activeTab="2"/>
+    <workbookView xWindow="15180" yWindow="150" windowWidth="5040" windowHeight="7470"/>
   </bookViews>
   <sheets>
     <sheet name="Main Test" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3692" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3945" uniqueCount="59">
   <si>
     <t/>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>in4</t>
-  </si>
-  <si>
-    <t>testRDir</t>
   </si>
   <si>
     <t>rexec</t>
@@ -239,6 +236,12 @@
   </si>
   <si>
     <t>0.8</t>
+  </si>
+  <si>
+    <t>testDir</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -469,10 +472,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="testdiagram.png">
+        <xdr:cNvPr id="10" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCFCBD86-DAF6-41BE-BC37-55A4D01BDD92}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9637BB30-BD20-4130-A887-5C300D0DBD3F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -494,7 +497,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2676525" y="4048125"/>
+          <a:off x="2676525" y="1133475"/>
           <a:ext cx="4572000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -941,7 +944,7 @@
   <sheetPr codeName="eingabe"/>
   <dimension ref="A1:O301"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
@@ -1027,7 +1030,7 @@
         <v>8</v>
       </c>
       <c r="O2" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -1069,7 +1072,7 @@
         <v>9</v>
       </c>
       <c r="O3" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -1111,7 +1114,7 @@
         <v>10</v>
       </c>
       <c r="O4" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -1153,7 +1156,7 @@
         <v>4</v>
       </c>
       <c r="O5" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -2399,7 +2402,10 @@
       </c>
       <c r="I48" s="7"/>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B49" s="11" t="s">
         <v>0</v>
       </c>
@@ -2423,7 +2429,10 @@
       </c>
       <c r="I49" s="7"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B50" s="11" t="s">
         <v>0</v>
       </c>
@@ -2447,7 +2456,10 @@
       </c>
       <c r="I50" s="7"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B51" s="11" t="s">
         <v>0</v>
       </c>
@@ -2470,7 +2482,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B52" s="11" t="s">
         <v>0</v>
       </c>
@@ -2493,7 +2508,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B53" s="11" t="s">
         <v>0</v>
       </c>
@@ -2516,7 +2534,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B54" s="11" t="s">
         <v>0</v>
       </c>
@@ -2539,7 +2560,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B55" s="11" t="s">
         <v>0</v>
       </c>
@@ -2562,7 +2586,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B56" s="11" t="s">
         <v>0</v>
       </c>
@@ -2585,7 +2612,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B57" s="11" t="s">
         <v>0</v>
       </c>
@@ -2608,7 +2638,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B58" s="11" t="s">
         <v>0</v>
       </c>
@@ -2631,7 +2664,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B59" s="11" t="s">
         <v>0</v>
       </c>
@@ -2654,7 +2690,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B60" s="11" t="s">
         <v>0</v>
       </c>
@@ -2677,7 +2716,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B61" s="11" t="s">
         <v>0</v>
       </c>
@@ -2700,7 +2742,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B62" s="11" t="s">
         <v>0</v>
       </c>
@@ -2723,7 +2768,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B63" s="11" t="s">
         <v>0</v>
       </c>
@@ -2746,7 +2794,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B64" s="11" t="s">
         <v>0</v>
       </c>
@@ -2769,7 +2820,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B65" s="11" t="s">
         <v>0</v>
       </c>
@@ -2792,7 +2846,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B66" s="11" t="s">
         <v>0</v>
       </c>
@@ -2815,7 +2872,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B67" s="11" t="s">
         <v>0</v>
       </c>
@@ -2838,7 +2898,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B68" s="11" t="s">
         <v>0</v>
       </c>
@@ -2861,7 +2924,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B69" s="11" t="s">
         <v>0</v>
       </c>
@@ -2884,7 +2950,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B70" s="11" t="s">
         <v>0</v>
       </c>
@@ -2907,7 +2976,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B71" s="11" t="s">
         <v>0</v>
       </c>
@@ -2930,7 +3002,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B72" s="11" t="s">
         <v>0</v>
       </c>
@@ -2953,7 +3028,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B73" s="11" t="s">
         <v>0</v>
       </c>
@@ -2976,7 +3054,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B74" s="11" t="s">
         <v>0</v>
       </c>
@@ -2999,7 +3080,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B75" s="11" t="s">
         <v>0</v>
       </c>
@@ -3022,7 +3106,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B76" s="11" t="s">
         <v>0</v>
       </c>
@@ -3045,7 +3132,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B77" s="11" t="s">
         <v>0</v>
       </c>
@@ -3068,7 +3158,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B78" s="11" t="s">
         <v>0</v>
       </c>
@@ -3091,7 +3184,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B79" s="11" t="s">
         <v>0</v>
       </c>
@@ -3114,7 +3210,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B80" s="11" t="s">
         <v>0</v>
       </c>
@@ -3137,7 +3236,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B81" s="11" t="s">
         <v>0</v>
       </c>
@@ -3160,7 +3262,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B82" s="11" t="s">
         <v>0</v>
       </c>
@@ -3183,7 +3288,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B83" s="11" t="s">
         <v>0</v>
       </c>
@@ -3206,7 +3314,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B84" s="11" t="s">
         <v>0</v>
       </c>
@@ -3229,7 +3340,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B85" s="11" t="s">
         <v>0</v>
       </c>
@@ -3252,7 +3366,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B86" s="11" t="s">
         <v>0</v>
       </c>
@@ -3275,7 +3392,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B87" s="11" t="s">
         <v>0</v>
       </c>
@@ -3298,7 +3418,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B88" s="11" t="s">
         <v>0</v>
       </c>
@@ -3321,7 +3444,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B89" s="11" t="s">
         <v>0</v>
       </c>
@@ -3344,7 +3470,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B90" s="11" t="s">
         <v>0</v>
       </c>
@@ -3367,7 +3496,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B91" s="11" t="s">
         <v>0</v>
       </c>
@@ -3390,7 +3522,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B92" s="11" t="s">
         <v>0</v>
       </c>
@@ -3413,7 +3548,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B93" s="11" t="s">
         <v>0</v>
       </c>
@@ -3436,7 +3574,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B94" s="11" t="s">
         <v>0</v>
       </c>
@@ -3459,7 +3600,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B95" s="11" t="s">
         <v>0</v>
       </c>
@@ -3482,7 +3626,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B96" s="11" t="s">
         <v>0</v>
       </c>
@@ -3505,7 +3652,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B97" s="11" t="s">
         <v>0</v>
       </c>
@@ -3528,7 +3678,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B98" s="11" t="s">
         <v>0</v>
       </c>
@@ -3551,7 +3704,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B99" s="11" t="s">
         <v>0</v>
       </c>
@@ -3574,7 +3730,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B100" s="11" t="s">
         <v>0</v>
       </c>
@@ -3597,7 +3756,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B101" s="11" t="s">
         <v>0</v>
       </c>
@@ -3620,7 +3782,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B102" s="11" t="s">
         <v>0</v>
       </c>
@@ -3643,7 +3808,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B103" s="11" t="s">
         <v>0</v>
       </c>
@@ -3666,7 +3834,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B104" s="11" t="s">
         <v>0</v>
       </c>
@@ -3689,7 +3860,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B105" s="11" t="s">
         <v>0</v>
       </c>
@@ -3712,7 +3886,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B106" s="11" t="s">
         <v>0</v>
       </c>
@@ -3735,7 +3912,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B107" s="11" t="s">
         <v>0</v>
       </c>
@@ -3758,7 +3938,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B108" s="11" t="s">
         <v>0</v>
       </c>
@@ -3781,7 +3964,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B109" s="11" t="s">
         <v>0</v>
       </c>
@@ -3804,7 +3990,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B110" s="11" t="s">
         <v>0</v>
       </c>
@@ -3827,7 +4016,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B111" s="11" t="s">
         <v>0</v>
       </c>
@@ -3850,7 +4042,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B112" s="11" t="s">
         <v>0</v>
       </c>
@@ -3873,7 +4068,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B113" s="11" t="s">
         <v>0</v>
       </c>
@@ -3896,7 +4094,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B114" s="11" t="s">
         <v>0</v>
       </c>
@@ -3919,7 +4120,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B115" s="11" t="s">
         <v>0</v>
       </c>
@@ -3942,7 +4146,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B116" s="11" t="s">
         <v>0</v>
       </c>
@@ -3965,7 +4172,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B117" s="11" t="s">
         <v>0</v>
       </c>
@@ -3988,7 +4198,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A118" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B118" s="11" t="s">
         <v>0</v>
       </c>
@@ -4011,7 +4224,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A119" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B119" s="11" t="s">
         <v>0</v>
       </c>
@@ -4034,7 +4250,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A120" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B120" s="11" t="s">
         <v>0</v>
       </c>
@@ -4057,7 +4276,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A121" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B121" s="11" t="s">
         <v>0</v>
       </c>
@@ -4080,7 +4302,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A122" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B122" s="11" t="s">
         <v>0</v>
       </c>
@@ -4103,7 +4328,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A123" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B123" s="11" t="s">
         <v>0</v>
       </c>
@@ -4126,7 +4354,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A124" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B124" s="11" t="s">
         <v>0</v>
       </c>
@@ -4149,7 +4380,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A125" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B125" s="11" t="s">
         <v>0</v>
       </c>
@@ -4172,7 +4406,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A126" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B126" s="11" t="s">
         <v>0</v>
       </c>
@@ -4195,7 +4432,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A127" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B127" s="11" t="s">
         <v>0</v>
       </c>
@@ -4218,7 +4458,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A128" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B128" s="11" t="s">
         <v>0</v>
       </c>
@@ -4241,7 +4484,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A129" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B129" s="11" t="s">
         <v>0</v>
       </c>
@@ -4264,7 +4510,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A130" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B130" s="11" t="s">
         <v>0</v>
       </c>
@@ -4287,7 +4536,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A131" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B131" s="11" t="s">
         <v>0</v>
       </c>
@@ -4310,7 +4562,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A132" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B132" s="11" t="s">
         <v>0</v>
       </c>
@@ -4333,7 +4588,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A133" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B133" s="11" t="s">
         <v>0</v>
       </c>
@@ -4356,7 +4614,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A134" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B134" s="11" t="s">
         <v>0</v>
       </c>
@@ -4379,7 +4640,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A135" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B135" s="11" t="s">
         <v>0</v>
       </c>
@@ -4402,7 +4666,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A136" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B136" s="11" t="s">
         <v>0</v>
       </c>
@@ -4425,7 +4692,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A137" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B137" s="11" t="s">
         <v>0</v>
       </c>
@@ -4448,7 +4718,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A138" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B138" s="11" t="s">
         <v>0</v>
       </c>
@@ -4471,7 +4744,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A139" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B139" s="11" t="s">
         <v>0</v>
       </c>
@@ -4494,7 +4770,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A140" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B140" s="11" t="s">
         <v>0</v>
       </c>
@@ -4517,7 +4796,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A141" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B141" s="11" t="s">
         <v>0</v>
       </c>
@@ -4540,7 +4822,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A142" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B142" s="11" t="s">
         <v>0</v>
       </c>
@@ -4563,7 +4848,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A143" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B143" s="11" t="s">
         <v>0</v>
       </c>
@@ -4586,7 +4874,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A144" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B144" s="11" t="s">
         <v>0</v>
       </c>
@@ -4609,7 +4900,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A145" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B145" s="11" t="s">
         <v>0</v>
       </c>
@@ -4632,7 +4926,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A146" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B146" s="11" t="s">
         <v>0</v>
       </c>
@@ -4655,7 +4952,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A147" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B147" s="11" t="s">
         <v>0</v>
       </c>
@@ -4678,7 +4978,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A148" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B148" s="11" t="s">
         <v>0</v>
       </c>
@@ -4701,7 +5004,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A149" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B149" s="11" t="s">
         <v>0</v>
       </c>
@@ -4724,7 +5030,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A150" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B150" s="11" t="s">
         <v>0</v>
       </c>
@@ -4747,7 +5056,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A151" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B151" s="11" t="s">
         <v>0</v>
       </c>
@@ -4770,7 +5082,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A152" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B152" s="11" t="s">
         <v>0</v>
       </c>
@@ -4793,7 +5108,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A153" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B153" s="11" t="s">
         <v>0</v>
       </c>
@@ -4816,7 +5134,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A154" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B154" s="11" t="s">
         <v>0</v>
       </c>
@@ -4839,7 +5160,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A155" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B155" s="11" t="s">
         <v>0</v>
       </c>
@@ -4862,7 +5186,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A156" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B156" s="11" t="s">
         <v>0</v>
       </c>
@@ -4885,7 +5212,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A157" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B157" s="11" t="s">
         <v>0</v>
       </c>
@@ -4908,7 +5238,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A158" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B158" s="11" t="s">
         <v>0</v>
       </c>
@@ -4931,7 +5264,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A159" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B159" s="11" t="s">
         <v>0</v>
       </c>
@@ -4954,7 +5290,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A160" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B160" s="11" t="s">
         <v>0</v>
       </c>
@@ -4977,7 +5316,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A161" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B161" s="11" t="s">
         <v>0</v>
       </c>
@@ -5000,7 +5342,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A162" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B162" s="11" t="s">
         <v>0</v>
       </c>
@@ -5023,7 +5368,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A163" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B163" s="11" t="s">
         <v>0</v>
       </c>
@@ -5046,7 +5394,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A164" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B164" s="11" t="s">
         <v>0</v>
       </c>
@@ -5069,7 +5420,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A165" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B165" s="11" t="s">
         <v>0</v>
       </c>
@@ -5092,7 +5446,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A166" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B166" s="11" t="s">
         <v>0</v>
       </c>
@@ -5115,7 +5472,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A167" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B167" s="11" t="s">
         <v>0</v>
       </c>
@@ -5138,7 +5498,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A168" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B168" s="11" t="s">
         <v>0</v>
       </c>
@@ -5161,7 +5524,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A169" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B169" s="11" t="s">
         <v>0</v>
       </c>
@@ -5184,7 +5550,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A170" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B170" s="11" t="s">
         <v>0</v>
       </c>
@@ -5207,7 +5576,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A171" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B171" s="11" t="s">
         <v>0</v>
       </c>
@@ -5230,7 +5602,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A172" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B172" s="11" t="s">
         <v>0</v>
       </c>
@@ -5253,7 +5628,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A173" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B173" s="11" t="s">
         <v>0</v>
       </c>
@@ -5276,7 +5654,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A174" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B174" s="11" t="s">
         <v>0</v>
       </c>
@@ -5299,7 +5680,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A175" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B175" s="11" t="s">
         <v>0</v>
       </c>
@@ -5322,7 +5706,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A176" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B176" s="11" t="s">
         <v>0</v>
       </c>
@@ -5345,7 +5732,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A177" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B177" s="11" t="s">
         <v>0</v>
       </c>
@@ -5368,7 +5758,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A178" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B178" s="11" t="s">
         <v>0</v>
       </c>
@@ -5391,7 +5784,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A179" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B179" s="11" t="s">
         <v>0</v>
       </c>
@@ -5414,7 +5810,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A180" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B180" s="11" t="s">
         <v>0</v>
       </c>
@@ -5437,7 +5836,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A181" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B181" s="11" t="s">
         <v>0</v>
       </c>
@@ -5460,7 +5862,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A182" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B182" s="11" t="s">
         <v>0</v>
       </c>
@@ -5483,7 +5888,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A183" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B183" s="11" t="s">
         <v>0</v>
       </c>
@@ -5506,7 +5914,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A184" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B184" s="11" t="s">
         <v>0</v>
       </c>
@@ -5529,7 +5940,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A185" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B185" s="11" t="s">
         <v>0</v>
       </c>
@@ -5552,7 +5966,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A186" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B186" s="11" t="s">
         <v>0</v>
       </c>
@@ -5575,7 +5992,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A187" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B187" s="11" t="s">
         <v>0</v>
       </c>
@@ -5598,7 +6018,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A188" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B188" s="11" t="s">
         <v>0</v>
       </c>
@@ -5621,7 +6044,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A189" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B189" s="11" t="s">
         <v>0</v>
       </c>
@@ -5644,7 +6070,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A190" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B190" s="11" t="s">
         <v>0</v>
       </c>
@@ -5667,7 +6096,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A191" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B191" s="11" t="s">
         <v>0</v>
       </c>
@@ -5690,7 +6122,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A192" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B192" s="11" t="s">
         <v>0</v>
       </c>
@@ -5713,7 +6148,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A193" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B193" s="11" t="s">
         <v>0</v>
       </c>
@@ -5736,7 +6174,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A194" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B194" s="11" t="s">
         <v>0</v>
       </c>
@@ -5759,7 +6200,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A195" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B195" s="11" t="s">
         <v>0</v>
       </c>
@@ -5782,7 +6226,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A196" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B196" s="11" t="s">
         <v>0</v>
       </c>
@@ -5805,7 +6252,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A197" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B197" s="11" t="s">
         <v>0</v>
       </c>
@@ -5828,7 +6278,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A198" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B198" s="11" t="s">
         <v>0</v>
       </c>
@@ -5851,7 +6304,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A199" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B199" s="11" t="s">
         <v>0</v>
       </c>
@@ -5874,7 +6330,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A200" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B200" s="11" t="s">
         <v>0</v>
       </c>
@@ -5897,7 +6356,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A201" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B201" s="11" t="s">
         <v>0</v>
       </c>
@@ -5920,7 +6382,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A202" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B202" s="11" t="s">
         <v>0</v>
       </c>
@@ -5943,7 +6408,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A203" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B203" s="11" t="s">
         <v>0</v>
       </c>
@@ -5966,7 +6434,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A204" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B204" s="11" t="s">
         <v>0</v>
       </c>
@@ -5989,7 +6460,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A205" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B205" s="11" t="s">
         <v>0</v>
       </c>
@@ -6012,7 +6486,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A206" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B206" s="11" t="s">
         <v>0</v>
       </c>
@@ -6035,7 +6512,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A207" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B207" s="11" t="s">
         <v>0</v>
       </c>
@@ -6058,7 +6538,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A208" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B208" s="11" t="s">
         <v>0</v>
       </c>
@@ -6081,7 +6564,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A209" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B209" s="11" t="s">
         <v>0</v>
       </c>
@@ -6104,7 +6590,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A210" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B210" s="11" t="s">
         <v>0</v>
       </c>
@@ -6127,7 +6616,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A211" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B211" s="11" t="s">
         <v>0</v>
       </c>
@@ -6150,7 +6642,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A212" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B212" s="11" t="s">
         <v>0</v>
       </c>
@@ -6173,7 +6668,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A213" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B213" s="11" t="s">
         <v>0</v>
       </c>
@@ -6196,7 +6694,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A214" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B214" s="11" t="s">
         <v>0</v>
       </c>
@@ -6219,7 +6720,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A215" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B215" s="11" t="s">
         <v>0</v>
       </c>
@@ -6242,7 +6746,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A216" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B216" s="11" t="s">
         <v>0</v>
       </c>
@@ -6265,7 +6772,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A217" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B217" s="11" t="s">
         <v>0</v>
       </c>
@@ -6288,7 +6798,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A218" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B218" s="11" t="s">
         <v>0</v>
       </c>
@@ -6311,7 +6824,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A219" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B219" s="11" t="s">
         <v>0</v>
       </c>
@@ -6334,7 +6850,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A220" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B220" s="11" t="s">
         <v>0</v>
       </c>
@@ -6357,7 +6876,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A221" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B221" s="11" t="s">
         <v>0</v>
       </c>
@@ -6380,7 +6902,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A222" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B222" s="11" t="s">
         <v>0</v>
       </c>
@@ -6403,7 +6928,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A223" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B223" s="11" t="s">
         <v>0</v>
       </c>
@@ -6426,7 +6954,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A224" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B224" s="11" t="s">
         <v>0</v>
       </c>
@@ -6449,7 +6980,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A225" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B225" s="11" t="s">
         <v>0</v>
       </c>
@@ -6472,7 +7006,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A226" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B226" s="11" t="s">
         <v>0</v>
       </c>
@@ -6495,7 +7032,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A227" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B227" s="11" t="s">
         <v>0</v>
       </c>
@@ -6518,7 +7058,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A228" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B228" s="11" t="s">
         <v>0</v>
       </c>
@@ -6541,7 +7084,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A229" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B229" s="11" t="s">
         <v>0</v>
       </c>
@@ -6564,7 +7110,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A230" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B230" s="11" t="s">
         <v>0</v>
       </c>
@@ -6587,7 +7136,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A231" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B231" s="11" t="s">
         <v>0</v>
       </c>
@@ -6610,7 +7162,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A232" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B232" s="11" t="s">
         <v>0</v>
       </c>
@@ -6633,7 +7188,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A233" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B233" s="11" t="s">
         <v>0</v>
       </c>
@@ -6656,7 +7214,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A234" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B234" s="11" t="s">
         <v>0</v>
       </c>
@@ -6679,7 +7240,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A235" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B235" s="11" t="s">
         <v>0</v>
       </c>
@@ -6702,7 +7266,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A236" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B236" s="11" t="s">
         <v>0</v>
       </c>
@@ -6725,7 +7292,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A237" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B237" s="11" t="s">
         <v>0</v>
       </c>
@@ -6748,7 +7318,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A238" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B238" s="11" t="s">
         <v>0</v>
       </c>
@@ -6771,7 +7344,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A239" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B239" s="11" t="s">
         <v>0</v>
       </c>
@@ -6794,7 +7370,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A240" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B240" s="11" t="s">
         <v>0</v>
       </c>
@@ -6817,7 +7396,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A241" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B241" s="11" t="s">
         <v>0</v>
       </c>
@@ -6840,7 +7422,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A242" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B242" s="11" t="s">
         <v>0</v>
       </c>
@@ -6863,7 +7448,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A243" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B243" s="11" t="s">
         <v>0</v>
       </c>
@@ -6886,7 +7474,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A244" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B244" s="11" t="s">
         <v>0</v>
       </c>
@@ -6909,7 +7500,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A245" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B245" s="11" t="s">
         <v>0</v>
       </c>
@@ -6932,7 +7526,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A246" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B246" s="11" t="s">
         <v>0</v>
       </c>
@@ -6955,7 +7552,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A247" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B247" s="11" t="s">
         <v>0</v>
       </c>
@@ -6978,7 +7578,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A248" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B248" s="11" t="s">
         <v>0</v>
       </c>
@@ -7001,7 +7604,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A249" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B249" s="11" t="s">
         <v>0</v>
       </c>
@@ -7024,7 +7630,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A250" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B250" s="11" t="s">
         <v>0</v>
       </c>
@@ -7047,7 +7656,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A251" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B251" s="11" t="s">
         <v>0</v>
       </c>
@@ -7070,7 +7682,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A252" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B252" s="11" t="s">
         <v>0</v>
       </c>
@@ -7093,7 +7708,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A253" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B253" s="11" t="s">
         <v>0</v>
       </c>
@@ -7116,7 +7734,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A254" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B254" s="11" t="s">
         <v>0</v>
       </c>
@@ -7139,7 +7760,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A255" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B255" s="11" t="s">
         <v>0</v>
       </c>
@@ -7162,7 +7786,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A256" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B256" s="11" t="s">
         <v>0</v>
       </c>
@@ -7185,7 +7812,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A257" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B257" s="11" t="s">
         <v>0</v>
       </c>
@@ -7208,7 +7838,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A258" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B258" s="11" t="s">
         <v>0</v>
       </c>
@@ -7231,7 +7864,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A259" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B259" s="11" t="s">
         <v>0</v>
       </c>
@@ -7254,7 +7890,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A260" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B260" s="11" t="s">
         <v>0</v>
       </c>
@@ -7277,7 +7916,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A261" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B261" s="11" t="s">
         <v>0</v>
       </c>
@@ -7300,7 +7942,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A262" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B262" s="11" t="s">
         <v>0</v>
       </c>
@@ -7323,7 +7968,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A263" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B263" s="11" t="s">
         <v>0</v>
       </c>
@@ -7346,7 +7994,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A264" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B264" s="11" t="s">
         <v>0</v>
       </c>
@@ -7369,7 +8020,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A265" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B265" s="11" t="s">
         <v>0</v>
       </c>
@@ -7392,7 +8046,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A266" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B266" s="11" t="s">
         <v>0</v>
       </c>
@@ -7415,7 +8072,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A267" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B267" s="11" t="s">
         <v>0</v>
       </c>
@@ -7438,7 +8098,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A268" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B268" s="11" t="s">
         <v>0</v>
       </c>
@@ -7461,7 +8124,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A269" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B269" s="11" t="s">
         <v>0</v>
       </c>
@@ -7484,7 +8150,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A270" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B270" s="11" t="s">
         <v>0</v>
       </c>
@@ -7507,7 +8176,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A271" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B271" s="11" t="s">
         <v>0</v>
       </c>
@@ -7530,7 +8202,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A272" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B272" s="11" t="s">
         <v>0</v>
       </c>
@@ -7553,7 +8228,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A273" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B273" s="11" t="s">
         <v>0</v>
       </c>
@@ -7576,7 +8254,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A274" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B274" s="11" t="s">
         <v>0</v>
       </c>
@@ -7599,7 +8280,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A275" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B275" s="11" t="s">
         <v>0</v>
       </c>
@@ -7622,7 +8306,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A276" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B276" s="11" t="s">
         <v>0</v>
       </c>
@@ -7645,7 +8332,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A277" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B277" s="11" t="s">
         <v>0</v>
       </c>
@@ -7668,7 +8358,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A278" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B278" s="11" t="s">
         <v>0</v>
       </c>
@@ -7691,7 +8384,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="279" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A279" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B279" s="11" t="s">
         <v>0</v>
       </c>
@@ -7714,7 +8410,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A280" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B280" s="11" t="s">
         <v>0</v>
       </c>
@@ -7737,7 +8436,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A281" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B281" s="11" t="s">
         <v>0</v>
       </c>
@@ -7760,7 +8462,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A282" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B282" s="11" t="s">
         <v>0</v>
       </c>
@@ -7783,7 +8488,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="283" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A283" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B283" s="11" t="s">
         <v>0</v>
       </c>
@@ -7806,7 +8514,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="284" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A284" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B284" s="11" t="s">
         <v>0</v>
       </c>
@@ -7829,7 +8540,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="285" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A285" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B285" s="11" t="s">
         <v>0</v>
       </c>
@@ -7852,7 +8566,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="286" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A286" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B286" s="11" t="s">
         <v>0</v>
       </c>
@@ -7875,7 +8592,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="287" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A287" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B287" s="11" t="s">
         <v>0</v>
       </c>
@@ -7898,7 +8618,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A288" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B288" s="11" t="s">
         <v>0</v>
       </c>
@@ -7921,7 +8644,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A289" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B289" s="11" t="s">
         <v>0</v>
       </c>
@@ -7944,7 +8670,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="290" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A290" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B290" s="11" t="s">
         <v>0</v>
       </c>
@@ -7967,7 +8696,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="291" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A291" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B291" s="11" t="s">
         <v>0</v>
       </c>
@@ -7990,7 +8722,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A292" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B292" s="11" t="s">
         <v>0</v>
       </c>
@@ -8013,7 +8748,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A293" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B293" s="11" t="s">
         <v>0</v>
       </c>
@@ -8036,7 +8774,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A294" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B294" s="11" t="s">
         <v>0</v>
       </c>
@@ -8059,7 +8800,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="295" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A295" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B295" s="11" t="s">
         <v>0</v>
       </c>
@@ -8082,7 +8826,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="296" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A296" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B296" s="11" t="s">
         <v>0</v>
       </c>
@@ -8105,7 +8852,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A297" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B297" s="11" t="s">
         <v>0</v>
       </c>
@@ -8128,7 +8878,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="298" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A298" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B298" s="11" t="s">
         <v>0</v>
       </c>
@@ -8151,7 +8904,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A299" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B299" s="11" t="s">
         <v>0</v>
       </c>
@@ -8174,7 +8930,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A300" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B300" s="11" t="s">
         <v>0</v>
       </c>
@@ -8197,7 +8956,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A301" s="11" t="s">
+        <v>58</v>
+      </c>
       <c r="B301" s="11" t="s">
         <v>0</v>
       </c>
@@ -8249,7 +9011,7 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B1" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -8260,7 +9022,7 @@
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -8271,7 +9033,7 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -8282,7 +9044,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -8293,7 +9055,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -8304,7 +9066,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -8315,7 +9077,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -8326,7 +9088,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -8337,7 +9099,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -8348,7 +9110,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -8359,7 +9121,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -8370,7 +9132,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -8381,7 +9143,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -8392,7 +9154,7 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
@@ -8403,7 +9165,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C15"/>
       <c r="D15"/>
@@ -8414,7 +9176,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
@@ -8425,7 +9187,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
@@ -8460,10 +9222,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -8505,7 +9267,7 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C23"/>
       <c r="D23"/>
@@ -8540,10 +9302,10 @@
     </row>
     <row r="26" spans="1:8" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
@@ -14692,7 +15454,7 @@
   <sheetPr codeName="eingabeToy"/>
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -14708,7 +15470,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>14</v>
@@ -14766,7 +15528,7 @@
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>8</v>
@@ -14803,7 +15565,7 @@
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -14836,7 +15598,7 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -14845,7 +15607,7 @@
         <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -14854,10 +15616,10 @@
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7"/>
       <c r="J7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" t="s">
         <v>19</v>
-      </c>
-      <c r="K7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -14876,7 +15638,7 @@
         <v>1</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -14885,7 +15647,7 @@
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -14894,7 +15656,7 @@
         <v>5</v>
       </c>
       <c r="K11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -14903,7 +15665,7 @@
         <v>7</v>
       </c>
       <c r="K12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -15045,7 +15807,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>14</v>
@@ -15071,10 +15833,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -15103,10 +15865,10 @@
     </row>
     <row r="3" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -15115,7 +15877,7 @@
         <v>500</v>
       </c>
       <c r="F3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -15139,7 +15901,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -15172,7 +15934,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -15180,7 +15942,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -15188,7 +15950,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -15219,7 +15981,7 @@
         <v>100</v>
       </c>
       <c r="F9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G9">
         <v>3</v>
@@ -15262,7 +16024,7 @@
         <v>300</v>
       </c>
       <c r="F11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G11">
         <v>3</v>

</xml_diff>

<commit_message>
New possibility to call Rscript definitions (for each sheet one menu button with scripts beneath) both shell and rdotnet can be toggled now
</commit_message>
<xml_diff>
--- a/testRAddin.xlsx
+++ b/testRAddin.xlsx
@@ -23,6 +23,7 @@
     <definedName name="R_Addin">'Main Test'!$J$1:$L$5</definedName>
     <definedName name="R_AddinAnotherDef" localSheetId="2">Test_OtherSheet!$J$7:$L$12</definedName>
     <definedName name="R_AddinAnotherDef">'Main Test'!$M$1:$O$5</definedName>
+    <definedName name="R_AddinErrorInDef">'Main Test'!$P$1:$R$5</definedName>
     <definedName name="R_AddinScriptCell" localSheetId="1">Test_scriptRng!$A$25:$C$29</definedName>
     <definedName name="R_AddinScriptRange" localSheetId="1">Test_scriptRng!$A$19:$C$23</definedName>
     <definedName name="scriptRange" localSheetId="1">Test_scriptRng!$B$1:$B$17</definedName>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3945" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3958" uniqueCount="60">
   <si>
     <t/>
   </si>
@@ -242,6 +243,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>testDirNonExisting</t>
   </si>
 </sst>
 </file>
@@ -472,10 +476,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="testdiagram.png">
+        <xdr:cNvPr id="8" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9637BB30-BD20-4130-A887-5C300D0DBD3F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{360028AC-2D26-4BDB-9C13-E9D851E55E7F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -582,10 +586,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="testdiagram.png">
+        <xdr:cNvPr id="10" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1F49981-5576-4A8B-A677-01A7DC2BA2DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -942,20 +946,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="eingabe"/>
-  <dimension ref="A1:O301"/>
+  <dimension ref="A1:R301"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+      <selection activeCell="J1" sqref="J1:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="8" width="4.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.5703125" customWidth="1"/>
-    <col min="18" max="18" width="86.5703125" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B1" s="11" t="s">
         <v>14</v>
       </c>
@@ -990,8 +994,15 @@
         <f ca="1">SUBSTITUTE(CELL("DATEINAME",O1),"[testRAddin.xlsx]Main Test","")</f>
         <v>C:\dev\RAddin\</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q1" t="str">
+        <f ca="1">SUBSTITUTE(CELL("DATEINAME",R1),"[testRAddin.xlsx]Main Test","")</f>
+        <v>C:\dev\RAddin\</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>0.29749999999999999</v>
       </c>
@@ -1032,8 +1043,17 @@
       <c r="O2" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>0.30690000000000001</v>
       </c>
@@ -1074,8 +1094,17 @@
       <c r="O3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>9</v>
+      </c>
+      <c r="R3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>1.04E-2</v>
       </c>
@@ -1116,8 +1145,17 @@
       <c r="O4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>10</v>
+      </c>
+      <c r="R4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>5.1000000000000004E-3</v>
       </c>
@@ -1158,8 +1196,17 @@
       <c r="O5" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>0.21249999999999999</v>
       </c>
@@ -1189,7 +1236,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>5.4999999999999997E-3</v>
       </c>
@@ -1219,7 +1266,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>8.5000000000000006E-3</v>
       </c>
@@ -1249,7 +1296,7 @@
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>1.1900000000000001E-2</v>
       </c>
@@ -1279,7 +1326,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2.3E-2</v>
       </c>
@@ -1309,7 +1356,7 @@
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>0.3836</v>
       </c>
@@ -1339,7 +1386,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>0.34520000000000001</v>
       </c>
@@ -1369,7 +1416,7 @@
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>1.4500000000000001E-2</v>
       </c>
@@ -1399,7 +1446,7 @@
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>1.4500000000000001E-2</v>
       </c>
@@ -1429,7 +1476,7 @@
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>1.0200000000000001E-2</v>
       </c>
@@ -1459,7 +1506,7 @@
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>0.29749999999999999</v>
       </c>
@@ -15455,7 +15502,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="J7" sqref="J7:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
scriptrng split into scriptcell/scriptrng to make it explicit (error handling) debug toggleButton instead of debug script def improved err message for Rdefinitions
</commit_message>
<xml_diff>
--- a/testRAddin.xlsx
+++ b/testRAddin.xlsx
@@ -18,6 +18,11 @@
     <sheet name="Test_RdotNet" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="Data" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
+    <definedName name="Data_1" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
+    <definedName name="Data_2" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
+    <definedName name="Data_3" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
+    <definedName name="Data_4" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
     <definedName name="R_Addin" localSheetId="2">Test_OtherSheet!$J$1:$L$5</definedName>
     <definedName name="R_Addin" localSheetId="3">Test_RdotNet!$A$1:$C$7</definedName>
     <definedName name="R_Addin">'Main Test'!$J$1:$L$5</definedName>
@@ -112,9 +117,6 @@
     <t>result:</t>
   </si>
   <si>
-    <t>debug</t>
-  </si>
-  <si>
     <t>scriptRng</t>
   </si>
   <si>
@@ -186,9 +188,6 @@
 png(filename="testdiagram.png")
 print(gplot)
 dev.off()</t>
-  </si>
-  <si>
-    <t>scriptRange</t>
   </si>
   <si>
     <t>Test_scriptRng!testdiagram</t>
@@ -345,6 +344,12 @@
   </si>
   <si>
     <t>0.0361</t>
+  </si>
+  <si>
+    <t>Test_scriptRng!scriptRange</t>
+  </si>
+  <si>
+    <t>scriptCell</t>
   </si>
 </sst>
 </file>
@@ -575,10 +580,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="testdiagram.png">
+        <xdr:cNvPr id="10" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FABE499-94AB-4CBC-AB12-AED4C00C5FC4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E89AAB81-170E-4AEB-9D5D-36EA56B638A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -630,10 +635,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="testdiagram.png">
+        <xdr:cNvPr id="3" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B501BFCF-F942-45E5-87E4-7C806D95B637}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFEA9CA9-F5BA-4B58-BC0B-1BDE8CC2F596}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -655,7 +660,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7324725" y="161925"/>
+          <a:off x="7572375" y="161925"/>
           <a:ext cx="4572000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1048,7 +1053,7 @@
   <dimension ref="A1:R50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1104,7 +1109,7 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B2" s="11">
         <v>0.29749999999999999</v>
@@ -1141,7 +1146,7 @@
         <v>8</v>
       </c>
       <c r="O2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>1</v>
@@ -1150,12 +1155,12 @@
         <v>8</v>
       </c>
       <c r="R2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B3" s="11">
         <v>0.30690000000000001</v>
@@ -1192,7 +1197,7 @@
         <v>9</v>
       </c>
       <c r="O3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>6</v>
@@ -1201,12 +1206,12 @@
         <v>9</v>
       </c>
       <c r="R3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B4" s="11">
         <v>1.04E-2</v>
@@ -1243,7 +1248,7 @@
         <v>10</v>
       </c>
       <c r="O4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>5</v>
@@ -1252,12 +1257,12 @@
         <v>10</v>
       </c>
       <c r="R4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B5" s="11">
         <v>5.1000000000000004E-3</v>
@@ -1294,7 +1299,7 @@
         <v>4</v>
       </c>
       <c r="O5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>7</v>
@@ -1303,12 +1308,12 @@
         <v>4</v>
       </c>
       <c r="R5" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B6" s="11">
         <v>0.21249999999999999</v>
@@ -1338,7 +1343,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B7" s="11">
         <v>5.4999999999999997E-3</v>
@@ -1368,7 +1373,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B8" s="11">
         <v>8.5000000000000006E-3</v>
@@ -1398,7 +1403,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" s="11">
         <v>1.1900000000000001E-2</v>
@@ -1428,7 +1433,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B10" s="11">
         <v>2.3E-2</v>
@@ -1458,7 +1463,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B11" s="11">
         <v>0.3836</v>
@@ -1488,7 +1493,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B12" s="11">
         <v>0.34520000000000001</v>
@@ -1518,7 +1523,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B13" s="11">
         <v>1.4500000000000001E-2</v>
@@ -1548,7 +1553,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B14" s="11">
         <v>1.4500000000000001E-2</v>
@@ -1578,7 +1583,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B15" s="11">
         <v>1.0200000000000001E-2</v>
@@ -1608,7 +1613,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" s="11">
         <v>0.29749999999999999</v>
@@ -1638,7 +1643,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B17" s="11">
         <v>0.29749999999999999</v>
@@ -1668,7 +1673,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B18" s="11">
         <v>7.7000000000000002E-3</v>
@@ -1698,7 +1703,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B19" s="11">
         <v>7.7000000000000002E-3</v>
@@ -1728,7 +1733,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B20" s="11">
         <v>1.1900000000000001E-2</v>
@@ -1758,7 +1763,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B21" s="11">
         <v>1.7000000000000001E-2</v>
@@ -1788,7 +1793,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B22" s="11">
         <v>1.9099999999999999E-2</v>
@@ -1818,7 +1823,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B23" s="11">
         <v>4.2500000000000003E-2</v>
@@ -1848,7 +1853,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B24" s="11">
         <v>3.8300000000000001E-2</v>
@@ -1878,7 +1883,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B25" s="11">
         <v>0.44500000000000001</v>
@@ -1908,7 +1913,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B26" s="11">
         <v>0.32979999999999998</v>
@@ -1938,7 +1943,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B27" s="11">
         <v>0.36049999999999999</v>
@@ -1968,7 +1973,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B28" s="11">
         <v>0.1918</v>
@@ -1998,7 +2003,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B29" s="11">
         <v>1.84E-2</v>
@@ -2028,7 +2033,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B30" s="11">
         <v>1.26E-2</v>
@@ -2058,7 +2063,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B31" s="11">
         <v>1.26E-2</v>
@@ -2088,7 +2093,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B32" s="11">
         <v>7.7000000000000002E-3</v>
@@ -2118,7 +2123,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B33" s="11">
         <v>0.34</v>
@@ -2146,7 +2151,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B34" s="11">
         <v>0.255</v>
@@ -2173,7 +2178,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B35" s="11">
         <v>0.255</v>
@@ -2200,7 +2205,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B36" s="11">
         <v>8.5000000000000006E-2</v>
@@ -2227,7 +2232,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B37" s="11">
         <v>1.15E-2</v>
@@ -2254,7 +2259,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B38" s="11">
         <v>6.6E-3</v>
@@ -2281,7 +2286,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B39" s="11">
         <v>6.6E-3</v>
@@ -2308,7 +2313,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B40" s="11">
         <v>2.7000000000000001E-3</v>
@@ -2335,7 +2340,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B41" s="11">
         <v>3.4000000000000002E-2</v>
@@ -2362,7 +2367,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B42" s="11">
         <v>1.7000000000000001E-2</v>
@@ -2389,7 +2394,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B43" s="11">
         <v>1.49E-2</v>
@@ -2416,7 +2421,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B44" s="11">
         <v>8.5000000000000006E-3</v>
@@ -2443,7 +2448,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B45" s="11">
         <v>5.9499999999999997E-2</v>
@@ -2470,7 +2475,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B46" s="11">
         <v>3.4000000000000002E-2</v>
@@ -2497,7 +2502,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B47" s="11">
         <v>3.61E-2</v>
@@ -2524,7 +2529,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B48" s="11">
         <v>1.7000000000000001E-2</v>
@@ -2569,22 +2574,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M302"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.7109375" style="11" customWidth="1"/>
     <col min="2" max="2" width="94.5703125" style="11" customWidth="1"/>
-    <col min="3" max="8" width="4.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" style="11" customWidth="1"/>
+    <col min="4" max="8" width="4.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.5703125" customWidth="1"/>
     <col min="18" max="18" width="86.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B1" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -2595,7 +2601,7 @@
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -2606,7 +2612,7 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -2617,7 +2623,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -2628,7 +2634,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -2639,7 +2645,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -2650,7 +2656,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -2661,7 +2667,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -2672,7 +2678,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -2683,7 +2689,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -2694,7 +2700,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -2705,7 +2711,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -2716,7 +2722,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -2727,7 +2733,7 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
@@ -2738,7 +2744,7 @@
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15"/>
       <c r="D15"/>
@@ -2749,7 +2755,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
@@ -2760,7 +2766,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
@@ -2795,10 +2801,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -2840,7 +2846,7 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23"/>
       <c r="D23"/>
@@ -2875,10 +2881,10 @@
     </row>
     <row r="26" spans="1:8" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
@@ -9028,7 +9034,7 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:L12"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9101,7 +9107,7 @@
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="3" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>8</v>
@@ -9138,7 +9144,7 @@
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -9171,7 +9177,7 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -9180,7 +9186,7 @@
         <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -9220,7 +9226,7 @@
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -9229,7 +9235,7 @@
         <v>5</v>
       </c>
       <c r="K11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -9238,7 +9244,7 @@
         <v>7</v>
       </c>
       <c r="K12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -9406,10 +9412,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -9438,10 +9444,10 @@
     </row>
     <row r="3" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -9450,7 +9456,7 @@
         <v>500</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -9474,7 +9480,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -9507,7 +9513,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -9515,7 +9521,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -9523,7 +9529,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -9554,7 +9560,7 @@
         <v>100</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G9">
         <v>3</v>
@@ -9597,7 +9603,7 @@
         <v>300</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G11">
         <v>3</v>

</xml_diff>

<commit_message>
improved Rdotnet arg storing and result retrieving
</commit_message>
<xml_diff>
--- a/testRAddin.xlsx
+++ b/testRAddin.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\RAddin\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="150" windowWidth="5040" windowHeight="7470"/>
+    <workbookView xWindow="15180" yWindow="150" windowWidth="5040" windowHeight="7470" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Main Test" sheetId="1" r:id="rId1"/>
@@ -24,7 +19,7 @@
     <definedName name="Data_3" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
     <definedName name="Data_4" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
     <definedName name="R_Addin" localSheetId="2">Test_OtherSheet!$J$1:$L$5</definedName>
-    <definedName name="R_Addin" localSheetId="3">Test_RdotNet!$A$1:$C$7</definedName>
+    <definedName name="R_Addin" localSheetId="3">Test_RdotNet!$A$1:$C$5</definedName>
     <definedName name="R_Addin">'Main Test'!$J$1:$L$5</definedName>
     <definedName name="R_AddinAnotherDef" localSheetId="2">Test_OtherSheet!$J$7:$L$12</definedName>
     <definedName name="R_AddinAnotherDef">'Main Test'!$M$1:$O$5</definedName>
@@ -40,16 +35,49 @@
     <definedName name="test_out">'Main Test'!$A$2:$A$49</definedName>
     <definedName name="test_out2" localSheetId="3">Test_RdotNet!$E$8</definedName>
     <definedName name="testdiagram" localSheetId="2">Test_OtherSheet!$J$17</definedName>
-    <definedName name="testdiagram" localSheetId="3">Test_RdotNet!$A$10</definedName>
+    <definedName name="testdiagram" localSheetId="3">Test_RdotNet!$A$8</definedName>
     <definedName name="testdiagram" localSheetId="1">Test_scriptRng!$D$2</definedName>
     <definedName name="testdiagram">'Main Test'!$J$8</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="test_out" type="6" refreshedVersion="0" background="1">
+    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\.\test_out.txt">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="test_out1" type="6" refreshedVersion="0" background="1">
+    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\.\test_out.txt" decimal="," thousands=".">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" name="test_out2" type="6" refreshedVersion="0" background="1">
+    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\.\test_out.txt" decimal="," thousands=".">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="test_out3" type="6" refreshedVersion="0" background="1">
+    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\\test_out.txt" decimal="," thousands=".">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1981" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="92">
   <si>
     <t/>
   </si>
@@ -193,9 +221,6 @@
     <t>Test_scriptRng!testdiagram</t>
   </si>
   <si>
-    <t>rpath</t>
-  </si>
-  <si>
     <t>Test_RdotNet!testdiagram</t>
   </si>
   <si>
@@ -214,28 +239,7 @@
     <t>Test_OtherSheet!testdiagram</t>
   </si>
   <si>
-    <t>C:\Program Files\Microsoft\MRO\R-3.3.2\bin</t>
-  </si>
-  <si>
     <t>Test_RdotNet!test_out2</t>
-  </si>
-  <si>
-    <t>0,5</t>
-  </si>
-  <si>
-    <t>0,9</t>
-  </si>
-  <si>
-    <t>library(ggplot2)
-header &lt;- unlist(test_in[1,]) # the first row will be the header
-test_in &lt;- test_in[-1,]          # removing the first row.
-colnames(test_in) &lt;-header
-test_out &lt;- c(1,2,3) # test_in[,1]+20
-test_out2 &lt;- test_in #data.frame(sapply(test_in, function(x) as.numeric(as.character(x))))
-#gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()</t>
-  </si>
-  <si>
-    <t>0.8</t>
   </si>
   <si>
     <t>testDir</t>
@@ -351,11 +355,33 @@
   <si>
     <t>scriptCell</t>
   </si>
+  <si>
+    <t>argc</t>
+  </si>
+  <si>
+    <t>dewey</t>
+  </si>
+  <si>
+    <t>huey</t>
+  </si>
+  <si>
+    <t>louie</t>
+  </si>
+  <si>
+    <t>library(ggplot2)
+test_out &lt;- c(1.5,2,3) # test_in[,1]+20
+test_out2 &lt;- test_in
+rownames(test_out2) &lt;- c("huey","dewey","louie")
+gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()
+png(filename="C:/dev/Raddin/trunk/testdiagram.png")
+print(gplot)
+dev.off()</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="\."/>
@@ -478,7 +504,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -502,7 +528,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -583,7 +608,7 @@
         <xdr:cNvPr id="10" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E89AAB81-170E-4AEB-9D5D-36EA56B638A6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E89AAB81-170E-4AEB-9D5D-36EA56B638A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -638,7 +663,7 @@
         <xdr:cNvPr id="3" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFEA9CA9-F5BA-4B58-BC0B-1BDE8CC2F596}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EFEA9CA9-F5BA-4B58-BC0B-1BDE8CC2F596}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -693,7 +718,7 @@
         <xdr:cNvPr id="10" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -728,10 +753,59 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3810000</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="testdiagram.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2266950"/>
+          <a:ext cx="4572000" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -769,9 +843,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -804,26 +878,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -856,26 +913,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1052,7 +1092,7 @@
   <sheetPr codeName="eingabe"/>
   <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
@@ -1097,19 +1137,19 @@
       </c>
       <c r="N1" t="str">
         <f ca="1">SUBSTITUTE(CELL("DATEINAME",O1),"[testRAddin.xlsx]Main Test","")</f>
-        <v>C:\dev\RAddin\</v>
+        <v>C:\dev\RAddin\trunk\</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="Q1" t="str">
         <f ca="1">SUBSTITUTE(CELL("DATEINAME",R1),"[testRAddin.xlsx]Main Test","")</f>
-        <v>C:\dev\RAddin\</v>
+        <v>C:\dev\RAddin\trunk\</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B2" s="11">
         <v>0.29749999999999999</v>
@@ -1146,7 +1186,7 @@
         <v>8</v>
       </c>
       <c r="O2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>1</v>
@@ -1155,12 +1195,12 @@
         <v>8</v>
       </c>
       <c r="R2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B3" s="11">
         <v>0.30690000000000001</v>
@@ -1197,7 +1237,7 @@
         <v>9</v>
       </c>
       <c r="O3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>6</v>
@@ -1206,12 +1246,12 @@
         <v>9</v>
       </c>
       <c r="R3" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="11" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B4" s="11">
         <v>1.04E-2</v>
@@ -1248,7 +1288,7 @@
         <v>10</v>
       </c>
       <c r="O4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>5</v>
@@ -1257,12 +1297,12 @@
         <v>10</v>
       </c>
       <c r="R4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B5" s="11">
         <v>5.1000000000000004E-3</v>
@@ -1299,7 +1339,7 @@
         <v>4</v>
       </c>
       <c r="O5" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>7</v>
@@ -1308,12 +1348,12 @@
         <v>4</v>
       </c>
       <c r="R5" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B6" s="11">
         <v>0.21249999999999999</v>
@@ -1343,7 +1383,7 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B7" s="11">
         <v>5.4999999999999997E-3</v>
@@ -1373,7 +1413,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B8" s="11">
         <v>8.5000000000000006E-3</v>
@@ -1403,7 +1443,7 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B9" s="11">
         <v>1.1900000000000001E-2</v>
@@ -1433,7 +1473,7 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B10" s="11">
         <v>2.3E-2</v>
@@ -1463,7 +1503,7 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B11" s="11">
         <v>0.3836</v>
@@ -1493,7 +1533,7 @@
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B12" s="11">
         <v>0.34520000000000001</v>
@@ -1523,7 +1563,7 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B13" s="11">
         <v>1.4500000000000001E-2</v>
@@ -1553,7 +1593,7 @@
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B14" s="11">
         <v>1.4500000000000001E-2</v>
@@ -1583,7 +1623,7 @@
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B15" s="11">
         <v>1.0200000000000001E-2</v>
@@ -1613,7 +1653,7 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B16" s="11">
         <v>0.29749999999999999</v>
@@ -1643,7 +1683,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="11" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B17" s="11">
         <v>0.29749999999999999</v>
@@ -1673,7 +1713,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B18" s="11">
         <v>7.7000000000000002E-3</v>
@@ -1703,7 +1743,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B19" s="11">
         <v>7.7000000000000002E-3</v>
@@ -1733,7 +1773,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B20" s="11">
         <v>1.1900000000000001E-2</v>
@@ -1763,7 +1803,7 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B21" s="11">
         <v>1.7000000000000001E-2</v>
@@ -1793,7 +1833,7 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B22" s="11">
         <v>1.9099999999999999E-2</v>
@@ -1823,7 +1863,7 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B23" s="11">
         <v>4.2500000000000003E-2</v>
@@ -1853,7 +1893,7 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B24" s="11">
         <v>3.8300000000000001E-2</v>
@@ -1883,7 +1923,7 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B25" s="11">
         <v>0.44500000000000001</v>
@@ -1913,7 +1953,7 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B26" s="11">
         <v>0.32979999999999998</v>
@@ -1943,7 +1983,7 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B27" s="11">
         <v>0.36049999999999999</v>
@@ -1973,7 +2013,7 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B28" s="11">
         <v>0.1918</v>
@@ -2003,7 +2043,7 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B29" s="11">
         <v>1.84E-2</v>
@@ -2033,7 +2073,7 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B30" s="11">
         <v>1.26E-2</v>
@@ -2063,7 +2103,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B31" s="11">
         <v>1.26E-2</v>
@@ -2093,7 +2133,7 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B32" s="11">
         <v>7.7000000000000002E-3</v>
@@ -2123,7 +2163,7 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B33" s="11">
         <v>0.34</v>
@@ -2151,7 +2191,7 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B34" s="11">
         <v>0.255</v>
@@ -2178,7 +2218,7 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B35" s="11">
         <v>0.255</v>
@@ -2205,7 +2245,7 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B36" s="11">
         <v>8.5000000000000006E-2</v>
@@ -2232,7 +2272,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B37" s="11">
         <v>1.15E-2</v>
@@ -2259,7 +2299,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B38" s="11">
         <v>6.6E-3</v>
@@ -2286,7 +2326,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B39" s="11">
         <v>6.6E-3</v>
@@ -2313,7 +2353,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B40" s="11">
         <v>2.7000000000000001E-3</v>
@@ -2340,7 +2380,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B41" s="11">
         <v>3.4000000000000002E-2</v>
@@ -2367,7 +2407,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B42" s="11">
         <v>1.7000000000000001E-2</v>
@@ -2394,7 +2434,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B43" s="11">
         <v>1.49E-2</v>
@@ -2421,7 +2461,7 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B44" s="11">
         <v>8.5000000000000006E-3</v>
@@ -2448,7 +2488,7 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B45" s="11">
         <v>5.9499999999999997E-2</v>
@@ -2475,7 +2515,7 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B46" s="11">
         <v>3.4000000000000002E-2</v>
@@ -2502,7 +2542,7 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B47" s="11">
         <v>3.61E-2</v>
@@ -2529,7 +2569,7 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B48" s="11">
         <v>1.7000000000000001E-2</v>
@@ -2574,8 +2614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M302"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:C23"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2804,7 +2844,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -2881,7 +2921,7 @@
     </row>
     <row r="26" spans="1:8" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>40</v>
@@ -9087,7 +9127,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="21">
         <v>0.5</v>
       </c>
       <c r="D2">
@@ -9120,7 +9160,7 @@
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="21">
         <v>0.6</v>
       </c>
       <c r="D3">
@@ -9144,7 +9184,7 @@
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -9154,7 +9194,7 @@
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="21">
         <v>0.8</v>
       </c>
       <c r="D4">
@@ -9177,7 +9217,7 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -9186,7 +9226,7 @@
         <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -9226,7 +9266,7 @@
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -9235,7 +9275,7 @@
         <v>5</v>
       </c>
       <c r="K11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -9244,7 +9284,7 @@
         <v>7</v>
       </c>
       <c r="K12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -9365,10 +9405,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9378,12 +9418,12 @@
     <col min="4" max="11" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>2</v>
+    <row r="1" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>3</v>
+        <v>91</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>21</v>
@@ -9410,12 +9450,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>49</v>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -9424,7 +9464,7 @@
         <v>100</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -9442,21 +9482,21 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="102" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" s="21" t="s">
-        <v>53</v>
+        <v>5</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>43</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3">
-        <v>500</v>
-      </c>
-      <c r="F3" t="s">
-        <v>54</v>
+        <v>68.56</v>
+      </c>
+      <c r="F3">
+        <v>1.68</v>
       </c>
       <c r="G3">
         <v>3</v>
@@ -9475,12 +9515,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>45</v>
+        <v>5</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>48</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -9508,62 +9548,46 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E8" t="s">
+      <c r="B5" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
         <v>14</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>15</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>16</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>17</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>11</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>12</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E9">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9">
         <v>100</v>
       </c>
-      <c r="F9" t="s">
-        <v>51</v>
-      </c>
       <c r="G9">
-        <v>3</v>
+        <v>0.6</v>
       </c>
       <c r="H9">
         <v>3</v>
@@ -9577,18 +9601,21 @@
       <c r="K9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E10">
-        <v>500</v>
+      <c r="L9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E10" t="s">
+        <v>88</v>
       </c>
       <c r="F10">
-        <v>0.8</v>
+        <v>68.56</v>
       </c>
       <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="I10">
+        <v>1.68</v>
+      </c>
+      <c r="H10">
         <v>3</v>
       </c>
       <c r="J10">
@@ -9597,18 +9624,21 @@
       <c r="K10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E11">
+      <c r="L10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11">
         <v>300</v>
       </c>
-      <c r="F11" t="s">
-        <v>52</v>
-      </c>
       <c r="G11">
-        <v>3</v>
-      </c>
-      <c r="I11">
+        <v>0.9</v>
+      </c>
+      <c r="H11">
         <v>3</v>
       </c>
       <c r="J11">
@@ -9617,8 +9647,12 @@
       <c r="K11">
         <v>3</v>
       </c>
+      <c r="L11">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed rHome/rPath improved rdotnet result fetching fixed results fetching in script way
</commit_message>
<xml_diff>
--- a/testRAddin.xlsx
+++ b/testRAddin.xlsx
@@ -24,6 +24,7 @@
     <definedName name="R_AddinAnotherDef" localSheetId="2">Test_OtherSheet!$J$7:$L$12</definedName>
     <definedName name="R_AddinAnotherDef">'Main Test'!$M$1:$O$5</definedName>
     <definedName name="R_AddinErrorInDef">'Main Test'!$P$1:$R$5</definedName>
+    <definedName name="R_AddinOtherPlot">Test_RdotNet!$A$39:$C$40</definedName>
     <definedName name="R_AddinScriptCell" localSheetId="1">Test_scriptRng!$A$25:$C$29</definedName>
     <definedName name="R_AddinScriptRange" localSheetId="1">Test_scriptRng!$A$19:$C$23</definedName>
     <definedName name="scriptRange" localSheetId="1">Test_scriptRng!$B$1:$B$17</definedName>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1977" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1987" uniqueCount="95">
   <si>
     <t/>
   </si>
@@ -359,20 +360,33 @@
     <t>argc</t>
   </si>
   <si>
-    <t>dewey</t>
+    <t>library(ggplot2)
+test_out &lt;- as.Date(c("2017-01-01","2017-01-02","2017-01-03"))+25569 # difference between 1/1/1900 and 1/1/1970 + MS error
+test_out2 &lt;- test_in
+rownames(test_out2) &lt;- c("huey","dewey","louie")
+gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()
+png(filename="C:/dev/Raddin/trunk/testdiagram.png")
+print(gplot)
+dev.off()</t>
   </si>
   <si>
     <t>huey</t>
   </si>
   <si>
+    <t>dewey</t>
+  </si>
+  <si>
     <t>louie</t>
   </si>
   <si>
+    <t>sdfs</t>
+  </si>
+  <si>
+    <t>ret</t>
+  </si>
+  <si>
     <t>library(ggplot2)
-test_out &lt;- c(1.5,2,3) # test_in[,1]+20
-test_out2 &lt;- test_in
-rownames(test_out2) &lt;- c("huey","dewey","louie")
-gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()
+gplot &lt;- ggplot(data = test_in, aes(x = in6, y = in7) ) + geom_point()
 png(filename="C:/dev/Raddin/trunk/testdiagram.png")
 print(gplot)
 dev.off()</t>
@@ -504,7 +518,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -533,6 +547,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Komma 2" xfId="3"/>
@@ -608,7 +623,7 @@
         <xdr:cNvPr id="10" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E89AAB81-170E-4AEB-9D5D-36EA56B638A6}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E89AAB81-170E-4AEB-9D5D-36EA56B638A6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -663,7 +678,7 @@
         <xdr:cNvPr id="3" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{EFEA9CA9-F5BA-4B58-BC0B-1BDE8CC2F596}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFEA9CA9-F5BA-4B58-BC0B-1BDE8CC2F596}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -718,7 +733,7 @@
         <xdr:cNvPr id="10" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -770,7 +785,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="testdiagram.png"/>
+        <xdr:cNvPr id="11" name="testdiagram.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -789,7 +804,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2266950"/>
+          <a:off x="0" y="2305050"/>
           <a:ext cx="4572000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9405,25 +9420,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="73.7109375" customWidth="1"/>
+    <col min="2" max="2" width="114.5703125" customWidth="1"/>
     <col min="3" max="3" width="5.140625" customWidth="1"/>
-    <col min="4" max="11" width="8.28515625" customWidth="1"/>
+    <col min="4" max="10" width="8.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>86</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>21</v>
@@ -9458,7 +9474,7 @@
         <v>44</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>42736</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -9470,10 +9486,10 @@
         <v>3</v>
       </c>
       <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
-        <v>3</v>
+        <v>0.1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>92</v>
       </c>
       <c r="J2" s="1">
         <v>3</v>
@@ -9490,7 +9506,7 @@
         <v>43</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>42737</v>
       </c>
       <c r="E3">
         <v>68.56</v>
@@ -9499,14 +9515,13 @@
         <v>1.68</v>
       </c>
       <c r="G3">
-        <v>3</v>
-      </c>
-      <c r="H3" t="str">
-        <f>IFERROR(IF(I3=0,CODE(RIGHT(Test_OtherSheet!#REF!,LEN(Test_OtherSheet!#REF!)-1))-64,CODE(Test_OtherSheet!#REF!)-64),"")</f>
-        <v/>
-      </c>
-      <c r="I3">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="H3">
+        <v>0.8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>92</v>
       </c>
       <c r="J3" s="1">
         <v>3</v>
@@ -9523,7 +9538,7 @@
         <v>48</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>42738</v>
       </c>
       <c r="E4">
         <v>300</v>
@@ -9532,14 +9547,13 @@
         <v>0.9</v>
       </c>
       <c r="G4">
-        <v>3</v>
-      </c>
-      <c r="H4" t="str">
-        <f>IFERROR(IF(I4=0,CODE(RIGHT(Test_OtherSheet!#REF!,LEN(Test_OtherSheet!#REF!)-1))-64,CODE(Test_OtherSheet!#REF!)-64),"")</f>
-        <v/>
-      </c>
-      <c r="I4">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>93</v>
       </c>
       <c r="J4" s="1">
         <v>3</v>
@@ -9593,10 +9607,10 @@
         <v>3</v>
       </c>
       <c r="I9">
-        <v>3</v>
-      </c>
-      <c r="J9">
-        <v>3</v>
+        <v>0.1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>92</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -9607,7 +9621,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="F10">
         <v>68.56</v>
@@ -9616,12 +9630,15 @@
         <v>1.68</v>
       </c>
       <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="J10">
-        <v>3</v>
-      </c>
-      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>0.8</v>
+      </c>
+      <c r="J10" t="s">
+        <v>92</v>
+      </c>
+      <c r="K10" s="22">
         <v>3</v>
       </c>
       <c r="L10">
@@ -9630,7 +9647,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F11">
         <v>300</v>
@@ -9639,16 +9656,38 @@
         <v>0.9</v>
       </c>
       <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="J11">
-        <v>3</v>
-      </c>
-      <c r="K11">
+        <v>5</v>
+      </c>
+      <c r="I11">
+        <v>5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>93</v>
+      </c>
+      <c r="K11" s="22">
         <v>3</v>
       </c>
       <c r="L11">
         <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K12" s="21"/>
+    </row>
+    <row r="39" spans="1:2" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug when OK on about box without any workbook open Doc improvements fixed ugly error message with scriptcell, when being incorrectly defined as scriptrng
</commit_message>
<xml_diff>
--- a/testRAddin.xlsx
+++ b/testRAddin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="150" windowWidth="5040" windowHeight="7470" activeTab="3"/>
+    <workbookView xWindow="15180" yWindow="150" windowWidth="5040" windowHeight="7470" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main Test" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1987" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1941" uniqueCount="62">
   <si>
     <t/>
   </si>
@@ -249,108 +249,6 @@
     <t>testDirNonExisting</t>
   </si>
   <si>
-    <t>0.2975</t>
-  </si>
-  <si>
-    <t>0.3069</t>
-  </si>
-  <si>
-    <t>0.0104</t>
-  </si>
-  <si>
-    <t>0.0051</t>
-  </si>
-  <si>
-    <t>0.2125</t>
-  </si>
-  <si>
-    <t>0.0055</t>
-  </si>
-  <si>
-    <t>0.0085</t>
-  </si>
-  <si>
-    <t>0.0119</t>
-  </si>
-  <si>
-    <t>0.023</t>
-  </si>
-  <si>
-    <t>0.3836</t>
-  </si>
-  <si>
-    <t>0.3452</t>
-  </si>
-  <si>
-    <t>0.0145</t>
-  </si>
-  <si>
-    <t>0.0102</t>
-  </si>
-  <si>
-    <t>0.0077</t>
-  </si>
-  <si>
-    <t>0.017</t>
-  </si>
-  <si>
-    <t>0.0191</t>
-  </si>
-  <si>
-    <t>0.0425</t>
-  </si>
-  <si>
-    <t>0.0383</t>
-  </si>
-  <si>
-    <t>0.445</t>
-  </si>
-  <si>
-    <t>0.3298</t>
-  </si>
-  <si>
-    <t>0.3605</t>
-  </si>
-  <si>
-    <t>0.1918</t>
-  </si>
-  <si>
-    <t>0.0184</t>
-  </si>
-  <si>
-    <t>0.0126</t>
-  </si>
-  <si>
-    <t>0.34</t>
-  </si>
-  <si>
-    <t>0.255</t>
-  </si>
-  <si>
-    <t>0.085</t>
-  </si>
-  <si>
-    <t>0.0115</t>
-  </si>
-  <si>
-    <t>0.0066</t>
-  </si>
-  <si>
-    <t>0.0027</t>
-  </si>
-  <si>
-    <t>0.034</t>
-  </si>
-  <si>
-    <t>0.0149</t>
-  </si>
-  <si>
-    <t>0.0595</t>
-  </si>
-  <si>
-    <t>0.0361</t>
-  </si>
-  <si>
     <t>Test_scriptRng!scriptRange</t>
   </si>
   <si>
@@ -391,6 +289,9 @@
 print(gplot)
 dev.off()</t>
   </si>
+  <si>
+    <t>-&gt; Attention, testdiagram appears in Main Test !!!</t>
+  </si>
 </sst>
 </file>
 
@@ -402,7 +303,7 @@
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -421,6 +322,18 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -518,7 +431,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -548,6 +461,8 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Komma 2" xfId="3"/>
@@ -620,13 +535,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="testdiagram.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E89AAB81-170E-4AEB-9D5D-36EA56B638A6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="7" name="testdiagram.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -645,7 +554,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2809875" y="1133475"/>
+          <a:off x="2676525" y="1133475"/>
           <a:ext cx="4572000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -659,61 +568,6 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>685800</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="testdiagram.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFEA9CA9-F5BA-4B58-BC0B-1BDE8CC2F596}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7572375" y="161925"/>
-          <a:ext cx="4572000" cy="4572000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -733,7 +587,7 @@
         <xdr:cNvPr id="10" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -768,7 +622,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1108,12 +962,12 @@
   <dimension ref="A1:R50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+      <selection activeCell="J1" sqref="J1:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="11" customWidth="1"/>
     <col min="2" max="8" width="4.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.5703125" customWidth="1"/>
     <col min="18" max="18" width="12.42578125" customWidth="1"/>
@@ -1163,8 +1017,8 @@
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>51</v>
+      <c r="A2" s="11">
+        <v>0.29749999999999999</v>
       </c>
       <c r="B2" s="11">
         <v>0.29749999999999999</v>
@@ -1214,8 +1068,8 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>52</v>
+      <c r="A3" s="11">
+        <v>0.30690000000000001</v>
       </c>
       <c r="B3" s="11">
         <v>0.30690000000000001</v>
@@ -1265,8 +1119,8 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>53</v>
+      <c r="A4" s="11">
+        <v>1.04E-2</v>
       </c>
       <c r="B4" s="11">
         <v>1.04E-2</v>
@@ -1316,8 +1170,8 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>54</v>
+      <c r="A5" s="11">
+        <v>5.1000000000000004E-3</v>
       </c>
       <c r="B5" s="11">
         <v>5.1000000000000004E-3</v>
@@ -1367,8 +1221,8 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>55</v>
+      <c r="A6" s="11">
+        <v>0.21249999999999999</v>
       </c>
       <c r="B6" s="11">
         <v>0.21249999999999999</v>
@@ -1397,8 +1251,8 @@
       <c r="M6" s="7"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>56</v>
+      <c r="A7" s="11">
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="B7" s="11">
         <v>5.4999999999999997E-3</v>
@@ -1427,8 +1281,8 @@
       <c r="M7" s="7"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
-        <v>57</v>
+      <c r="A8" s="11">
+        <v>8.5000000000000006E-3</v>
       </c>
       <c r="B8" s="11">
         <v>8.5000000000000006E-3</v>
@@ -1457,8 +1311,8 @@
       <c r="M8" s="7"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>58</v>
+      <c r="A9" s="11">
+        <v>1.1900000000000001E-2</v>
       </c>
       <c r="B9" s="11">
         <v>1.1900000000000001E-2</v>
@@ -1487,8 +1341,8 @@
       <c r="M9" s="7"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>59</v>
+      <c r="A10" s="11">
+        <v>2.3E-2</v>
       </c>
       <c r="B10" s="11">
         <v>2.3E-2</v>
@@ -1517,8 +1371,8 @@
       <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>60</v>
+      <c r="A11" s="11">
+        <v>0.3836</v>
       </c>
       <c r="B11" s="11">
         <v>0.3836</v>
@@ -1547,8 +1401,8 @@
       <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>61</v>
+      <c r="A12" s="11">
+        <v>0.34520000000000001</v>
       </c>
       <c r="B12" s="11">
         <v>0.34520000000000001</v>
@@ -1577,8 +1431,8 @@
       <c r="M12" s="7"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
-        <v>62</v>
+      <c r="A13" s="11">
+        <v>1.4500000000000001E-2</v>
       </c>
       <c r="B13" s="11">
         <v>1.4500000000000001E-2</v>
@@ -1607,8 +1461,8 @@
       <c r="M13" s="7"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
-        <v>62</v>
+      <c r="A14" s="11">
+        <v>1.4500000000000001E-2</v>
       </c>
       <c r="B14" s="11">
         <v>1.4500000000000001E-2</v>
@@ -1637,8 +1491,8 @@
       <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
-        <v>63</v>
+      <c r="A15" s="11">
+        <v>1.0200000000000001E-2</v>
       </c>
       <c r="B15" s="11">
         <v>1.0200000000000001E-2</v>
@@ -1667,8 +1521,8 @@
       <c r="M15" s="7"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
-        <v>51</v>
+      <c r="A16" s="11">
+        <v>0.29749999999999999</v>
       </c>
       <c r="B16" s="11">
         <v>0.29749999999999999</v>
@@ -1697,8 +1551,8 @@
       <c r="M16" s="7"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
-        <v>51</v>
+      <c r="A17" s="11">
+        <v>0.29749999999999999</v>
       </c>
       <c r="B17" s="11">
         <v>0.29749999999999999</v>
@@ -1727,8 +1581,8 @@
       <c r="M17" s="7"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
-        <v>64</v>
+      <c r="A18" s="11">
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="B18" s="11">
         <v>7.7000000000000002E-3</v>
@@ -1757,8 +1611,8 @@
       <c r="M18" s="7"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
-        <v>64</v>
+      <c r="A19" s="11">
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="B19" s="11">
         <v>7.7000000000000002E-3</v>
@@ -1787,8 +1641,8 @@
       <c r="M19" s="7"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
-        <v>58</v>
+      <c r="A20" s="11">
+        <v>1.1900000000000001E-2</v>
       </c>
       <c r="B20" s="11">
         <v>1.1900000000000001E-2</v>
@@ -1817,8 +1671,8 @@
       <c r="M20" s="7"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
-        <v>65</v>
+      <c r="A21" s="11">
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="B21" s="11">
         <v>1.7000000000000001E-2</v>
@@ -1847,8 +1701,8 @@
       <c r="M21" s="7"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
-        <v>66</v>
+      <c r="A22" s="11">
+        <v>1.9099999999999999E-2</v>
       </c>
       <c r="B22" s="11">
         <v>1.9099999999999999E-2</v>
@@ -1877,8 +1731,8 @@
       <c r="M22" s="7"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>67</v>
+      <c r="A23" s="11">
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="B23" s="11">
         <v>4.2500000000000003E-2</v>
@@ -1907,8 +1761,8 @@
       <c r="M23" s="7"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
-        <v>68</v>
+      <c r="A24" s="11">
+        <v>3.8300000000000001E-2</v>
       </c>
       <c r="B24" s="11">
         <v>3.8300000000000001E-2</v>
@@ -1937,8 +1791,8 @@
       <c r="M24" s="7"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
-        <v>69</v>
+      <c r="A25" s="11">
+        <v>0.44500000000000001</v>
       </c>
       <c r="B25" s="11">
         <v>0.44500000000000001</v>
@@ -1967,8 +1821,8 @@
       <c r="M25" s="7"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
-        <v>70</v>
+      <c r="A26" s="11">
+        <v>0.32979999999999998</v>
       </c>
       <c r="B26" s="11">
         <v>0.32979999999999998</v>
@@ -1997,8 +1851,8 @@
       <c r="M26" s="7"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
-        <v>71</v>
+      <c r="A27" s="11">
+        <v>0.36049999999999999</v>
       </c>
       <c r="B27" s="11">
         <v>0.36049999999999999</v>
@@ -2027,8 +1881,8 @@
       <c r="M27" s="7"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
-        <v>72</v>
+      <c r="A28" s="11">
+        <v>0.1918</v>
       </c>
       <c r="B28" s="11">
         <v>0.1918</v>
@@ -2057,8 +1911,8 @@
       <c r="M28" s="7"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
-        <v>73</v>
+      <c r="A29" s="11">
+        <v>1.84E-2</v>
       </c>
       <c r="B29" s="11">
         <v>1.84E-2</v>
@@ -2087,8 +1941,8 @@
       <c r="M29" s="7"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>74</v>
+      <c r="A30" s="11">
+        <v>1.26E-2</v>
       </c>
       <c r="B30" s="11">
         <v>1.26E-2</v>
@@ -2117,8 +1971,8 @@
       <c r="M30" s="7"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
-        <v>74</v>
+      <c r="A31" s="11">
+        <v>1.26E-2</v>
       </c>
       <c r="B31" s="11">
         <v>1.26E-2</v>
@@ -2147,8 +2001,8 @@
       <c r="M31" s="7"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="11" t="s">
-        <v>64</v>
+      <c r="A32" s="11">
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="B32" s="11">
         <v>7.7000000000000002E-3</v>
@@ -2177,8 +2031,8 @@
       <c r="M32" s="7"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
-        <v>75</v>
+      <c r="A33" s="11">
+        <v>0.34</v>
       </c>
       <c r="B33" s="11">
         <v>0.34</v>
@@ -2205,8 +2059,8 @@
       <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
-        <v>76</v>
+      <c r="A34" s="11">
+        <v>0.255</v>
       </c>
       <c r="B34" s="11">
         <v>0.255</v>
@@ -2232,8 +2086,8 @@
       <c r="I34" s="7"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
-        <v>76</v>
+      <c r="A35" s="11">
+        <v>0.255</v>
       </c>
       <c r="B35" s="11">
         <v>0.255</v>
@@ -2259,8 +2113,8 @@
       <c r="I35" s="7"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
-        <v>77</v>
+      <c r="A36" s="11">
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="B36" s="11">
         <v>8.5000000000000006E-2</v>
@@ -2286,8 +2140,8 @@
       <c r="I36" s="7"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
-        <v>78</v>
+      <c r="A37" s="11">
+        <v>1.15E-2</v>
       </c>
       <c r="B37" s="11">
         <v>1.15E-2</v>
@@ -2313,8 +2167,8 @@
       <c r="I37" s="7"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="11" t="s">
-        <v>79</v>
+      <c r="A38" s="11">
+        <v>6.6E-3</v>
       </c>
       <c r="B38" s="11">
         <v>6.6E-3</v>
@@ -2340,8 +2194,8 @@
       <c r="I38" s="7"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
-        <v>79</v>
+      <c r="A39" s="11">
+        <v>6.6E-3</v>
       </c>
       <c r="B39" s="11">
         <v>6.6E-3</v>
@@ -2367,8 +2221,8 @@
       <c r="I39" s="7"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
-        <v>80</v>
+      <c r="A40" s="11">
+        <v>2.7000000000000001E-3</v>
       </c>
       <c r="B40" s="11">
         <v>2.7000000000000001E-3</v>
@@ -2394,8 +2248,8 @@
       <c r="I40" s="7"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>81</v>
+      <c r="A41" s="11">
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="B41" s="11">
         <v>3.4000000000000002E-2</v>
@@ -2421,8 +2275,8 @@
       <c r="I41" s="7"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
-        <v>65</v>
+      <c r="A42" s="11">
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="B42" s="11">
         <v>1.7000000000000001E-2</v>
@@ -2448,8 +2302,8 @@
       <c r="I42" s="7"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
-        <v>82</v>
+      <c r="A43" s="11">
+        <v>1.49E-2</v>
       </c>
       <c r="B43" s="11">
         <v>1.49E-2</v>
@@ -2475,8 +2329,8 @@
       <c r="I43" s="7"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="11" t="s">
-        <v>57</v>
+      <c r="A44" s="11">
+        <v>8.5000000000000006E-3</v>
       </c>
       <c r="B44" s="11">
         <v>8.5000000000000006E-3</v>
@@ -2502,8 +2356,8 @@
       <c r="I44" s="7"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
-        <v>83</v>
+      <c r="A45" s="11">
+        <v>5.9499999999999997E-2</v>
       </c>
       <c r="B45" s="11">
         <v>5.9499999999999997E-2</v>
@@ -2529,8 +2383,8 @@
       <c r="I45" s="7"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
-        <v>81</v>
+      <c r="A46" s="11">
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="B46" s="11">
         <v>3.4000000000000002E-2</v>
@@ -2556,8 +2410,8 @@
       <c r="I46" s="7"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
-        <v>84</v>
+      <c r="A47" s="11">
+        <v>3.61E-2</v>
       </c>
       <c r="B47" s="11">
         <v>3.61E-2</v>
@@ -2583,8 +2437,8 @@
       <c r="I47" s="7"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="11" t="s">
-        <v>65</v>
+      <c r="A48" s="11">
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="B48" s="11">
         <v>1.7000000000000001E-2</v>
@@ -2629,8 +2483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M302"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2859,7 +2713,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -2936,13 +2790,12 @@
     </row>
     <row r="26" spans="1:8" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>40</v>
       </c>
       <c r="C26"/>
-      <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26"/>
@@ -2956,7 +2809,7 @@
         <v>9</v>
       </c>
       <c r="C27"/>
-      <c r="D27"/>
+      <c r="D27" s="23"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
@@ -2990,9 +2843,11 @@
       <c r="G29"/>
       <c r="H29"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A30"/>
-      <c r="B30"/>
+      <c r="B30" s="24" t="s">
+        <v>61</v>
+      </c>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
@@ -9079,7 +8934,6 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;Z&amp;F&amp;A</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -9422,8 +9276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9436,10 +9290,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>88</v>
+        <v>54</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>21</v>
@@ -9468,7 +9322,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>87</v>
+        <v>53</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>44</v>
@@ -9489,7 +9343,7 @@
         <v>0.1</v>
       </c>
       <c r="I2" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="J2" s="1">
         <v>3</v>
@@ -9521,7 +9375,7 @@
         <v>0.8</v>
       </c>
       <c r="I3" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="J3" s="1">
         <v>3</v>
@@ -9553,7 +9407,7 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="J4" s="1">
         <v>3</v>
@@ -9595,7 +9449,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>89</v>
+        <v>55</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -9610,7 +9464,7 @@
         <v>0.1</v>
       </c>
       <c r="J9" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -9621,7 +9475,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="F10">
         <v>68.56</v>
@@ -9636,7 +9490,7 @@
         <v>0.8</v>
       </c>
       <c r="J10" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="K10" s="22">
         <v>3</v>
@@ -9647,7 +9501,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="F11">
         <v>300</v>
@@ -9662,7 +9516,7 @@
         <v>5</v>
       </c>
       <c r="J11" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="K11" s="22">
         <v>3</v>
@@ -9676,10 +9530,10 @@
     </row>
     <row r="39" spans="1:2" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>86</v>
+        <v>52</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
removed explicit TextFilePlatform setting in tabular data writing (takes default platform parameter now) changed encoding of sriptrng/scriptcell text from unicode to default encoding (usually ANSI) as it lead to problems with special characters
</commit_message>
<xml_diff>
--- a/testRAddin.xlsx
+++ b/testRAddin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="15180" yWindow="150" windowWidth="5040" windowHeight="7470" activeTab="1"/>
+    <workbookView xWindow="15180" yWindow="150" windowWidth="5040" windowHeight="7470"/>
   </bookViews>
   <sheets>
     <sheet name="Main Test" sheetId="1" r:id="rId1"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1941" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1944" uniqueCount="65">
   <si>
     <t/>
   </si>
@@ -292,6 +292,15 @@
   <si>
     <t>-&gt; Attention, testdiagram appears in Main Test !!!</t>
   </si>
+  <si>
+    <t>ä</t>
+  </si>
+  <si>
+    <t>ö</t>
+  </si>
+  <si>
+    <t>ß</t>
+  </si>
 </sst>
 </file>
 
@@ -431,7 +440,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -463,6 +472,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Komma 2" xfId="3"/>
@@ -587,7 +597,7 @@
         <xdr:cNvPr id="10" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -961,8 +971,8 @@
   <sheetPr codeName="eingabe"/>
   <dimension ref="A1:R50"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2452,14 +2462,14 @@
       <c r="E48" s="11">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="F48" s="11">
-        <v>2.3E-2</v>
-      </c>
-      <c r="G48" s="11">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="H48" s="11">
-        <v>2.3E-2</v>
+      <c r="F48" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="G48" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="H48" s="25" t="s">
+        <v>62</v>
       </c>
       <c r="I48" s="7"/>
     </row>
@@ -2483,8 +2493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M302"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>